<commit_message>
ajustes finais para a nova versao
</commit_message>
<xml_diff>
--- a/files/downloads/excel/organizese.xlsx
+++ b/files/downloads/excel/organizese.xlsx
@@ -468,7 +468,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2021-03-31</t>
+          <t>2021-04-28</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -478,22 +478,22 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>saida</t>
+          <t>entrada</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>50</v>
+        <v>21.21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Banco</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2021-03-10</t>
+          <t>2021-04-27</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -503,11 +503,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>entrada</t>
+          <t>saida</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1000</v>
+        <v>178.8</v>
       </c>
     </row>
     <row r="4">
@@ -520,7 +520,7 @@
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>950</v>
+        <v>-157.59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>